<commit_message>
Fix translations not working on m_logs table, I had writen prompt.title.es instead of prompt.title.text.es in the xlsx
</commit_message>
<xml_diff>
--- a/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
+++ b/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">display.prompt.text</t>
   </si>
   <si>
-    <t xml:space="preserve">display.prompt.es</t>
+    <t xml:space="preserve">display.prompt.text.es</t>
   </si>
   <si>
     <t xml:space="preserve">begin screen</t>
@@ -462,7 +462,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fix translation I had forgotten to write in the xlsx
</commit_message>
<xml_diff>
--- a/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
+++ b/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -71,6 +71,9 @@
     <t xml:space="preserve">Enter the ID of the refrigerator</t>
   </si>
   <si>
+    <t xml:space="preserve">Por favor entre el ID del frigorífico</t>
+  </si>
+  <si>
     <t xml:space="preserve">if</t>
   </si>
   <si>
@@ -81,9 +84,6 @@
   </si>
   <si>
     <t xml:space="preserve">refrigerator_row_id_fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Por favor entre el ID del frigorífico</t>
   </si>
   <si>
     <t xml:space="preserve">end if</t>
@@ -462,7 +462,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -538,11 +538,13 @@
       <c r="H3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -557,19 +559,19 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>14</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,7 +741,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Remove guids from various views
</commit_message>
<xml_diff>
--- a/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
+++ b/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -53,9 +53,15 @@
     <t xml:space="preserve">display.prompt.text.es</t>
   </si>
   <si>
+    <t xml:space="preserve">required</t>
+  </si>
+  <si>
     <t xml:space="preserve">begin screen</t>
   </si>
   <si>
+    <t xml:space="preserve">if</t>
+  </si>
+  <si>
     <t xml:space="preserve">string</t>
   </si>
   <si>
@@ -74,85 +80,76 @@
     <t xml:space="preserve">Por favor entre el ID del frigorífico</t>
   </si>
   <si>
-    <t xml:space="preserve">if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one_dropdown</t>
+    <t xml:space="preserve">end if</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_serviced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Serviced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de Servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the date of service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter any extra notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas extras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice_list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">query_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">query_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_form_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linked_table_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selectionArgs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newRowInitialElementKeyToValueMap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openRowInitialElementKeyToValueMap</t>
   </si>
   <si>
     <t xml:space="preserve">refrigerator_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">refrigerator_row_id_fake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end if</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_serviced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Serviced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de Servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the date of service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter any extra notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notas extras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice_list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">query_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">query_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_form_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linked_table_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">selectionArgs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newRowInitialElementKeyToValueMap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">openRowInitialElementKeyToValueMap</t>
   </si>
   <si>
     <t xml:space="preserve">linked_table</t>
@@ -459,10 +456,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -505,10 +502,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -520,119 +520,112 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="H4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>15</v>
-      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="I10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="3" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="I11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>21</v>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -667,10 +660,10 @@
   <sheetData>
     <row r="2" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -715,54 +708,54 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -799,10 +792,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>5</v>
@@ -811,42 +804,42 @@
         <v>6</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>20170717</v>
@@ -854,32 +847,32 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -911,70 +904,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="C4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Remove guids from m_logs detail
</commit_message>
<xml_diff>
--- a/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
+++ b/app/config/tables/m_logs/forms/m_logs/maintenance_logs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -83,40 +83,40 @@
     <t xml:space="preserve">end if</t>
   </si>
   <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_serviced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date Serviced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de Servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter the date of service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de servicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter any extra notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notas extras</t>
+  </si>
+  <si>
     <t xml:space="preserve">end screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date_serviced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date Serviced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de Servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the date of service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de servicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter any extra notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notas extras</t>
   </si>
   <si>
     <t xml:space="preserve">choice_list_name</t>
@@ -456,10 +456,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,59 +573,49 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="F7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="I7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -850,7 +840,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>